<commit_message>
Fixed: - issue feedback Added: - pheConfig
</commit_message>
<xml_diff>
--- a/dev/cuahang.xlsx
+++ b/dev/cuahang.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25520" windowHeight="15540"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25520" windowHeight="15540" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Phế khách mới" sheetId="3" r:id="rId1"/>
+    <sheet name="Phế khách cũ" sheetId="4" state="hidden" r:id="rId1"/>
+    <sheet name="Phế khách mới" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="1">
   <si>
     <t>money</t>
   </si>
@@ -423,6 +424,1168 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>15</v>
+      </c>
+      <c r="C1" s="1">
+        <v>20</v>
+      </c>
+      <c r="D1" s="1">
+        <v>21</v>
+      </c>
+      <c r="E1" s="1">
+        <v>22</v>
+      </c>
+      <c r="F1" s="1">
+        <v>24</v>
+      </c>
+      <c r="G1" s="1">
+        <v>25</v>
+      </c>
+      <c r="H1" s="1">
+        <v>26</v>
+      </c>
+      <c r="I1" s="1">
+        <v>27</v>
+      </c>
+      <c r="J1" s="1">
+        <v>30</v>
+      </c>
+      <c r="K1" s="1">
+        <v>31</v>
+      </c>
+      <c r="L1" s="1">
+        <v>32</v>
+      </c>
+      <c r="M1" s="1">
+        <v>33</v>
+      </c>
+      <c r="N1" s="1">
+        <v>40</v>
+      </c>
+      <c r="O1" s="1">
+        <v>41</v>
+      </c>
+      <c r="P1" s="1">
+        <v>42</v>
+      </c>
+      <c r="Q1" s="1">
+        <v>43</v>
+      </c>
+      <c r="R1" s="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="B2" s="2">
+        <f t="shared" ref="B2:R2" si="0">0.5*B3</f>
+        <v>10</v>
+      </c>
+      <c r="C2" s="2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="D2" s="2">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="E2" s="2">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="F2" s="2">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="G2" s="2">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="H2" s="2">
+        <f t="shared" si="0"/>
+        <v>15.5</v>
+      </c>
+      <c r="I2" s="2">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="J2" s="2">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="K2" s="2">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="L2" s="2">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="M2" s="2">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="N2" s="2">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="O2" s="2">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="P2" s="2">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="Q2" s="2">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="R2" s="2">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>2000</v>
+      </c>
+      <c r="B3" s="2">
+        <v>20</v>
+      </c>
+      <c r="C3" s="2">
+        <v>24</v>
+      </c>
+      <c r="D3" s="2">
+        <v>26</v>
+      </c>
+      <c r="E3" s="2">
+        <v>26</v>
+      </c>
+      <c r="F3" s="2">
+        <v>30</v>
+      </c>
+      <c r="G3" s="2">
+        <v>30</v>
+      </c>
+      <c r="H3" s="2">
+        <v>31</v>
+      </c>
+      <c r="I3" s="2">
+        <v>32</v>
+      </c>
+      <c r="J3" s="2">
+        <v>36</v>
+      </c>
+      <c r="K3" s="2">
+        <v>38</v>
+      </c>
+      <c r="L3" s="2">
+        <v>38</v>
+      </c>
+      <c r="M3" s="2">
+        <v>40</v>
+      </c>
+      <c r="N3" s="2">
+        <v>40</v>
+      </c>
+      <c r="O3" s="2">
+        <v>40</v>
+      </c>
+      <c r="P3" s="2">
+        <v>40</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>40</v>
+      </c>
+      <c r="R3" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>2500</v>
+      </c>
+      <c r="B4" s="2">
+        <v>25</v>
+      </c>
+      <c r="C4" s="2">
+        <v>30</v>
+      </c>
+      <c r="D4" s="2">
+        <v>32</v>
+      </c>
+      <c r="E4" s="2">
+        <v>32</v>
+      </c>
+      <c r="F4" s="2">
+        <v>37</v>
+      </c>
+      <c r="G4" s="2">
+        <v>37</v>
+      </c>
+      <c r="H4" s="2">
+        <v>38</v>
+      </c>
+      <c r="I4" s="2">
+        <v>40</v>
+      </c>
+      <c r="J4" s="2">
+        <f>(0.018*M4)/0.02</f>
+        <v>44.999999999999993</v>
+      </c>
+      <c r="K4" s="2">
+        <v>47</v>
+      </c>
+      <c r="L4" s="2">
+        <v>47</v>
+      </c>
+      <c r="M4" s="2">
+        <v>50</v>
+      </c>
+      <c r="N4" s="2">
+        <v>50</v>
+      </c>
+      <c r="O4" s="2">
+        <v>50</v>
+      </c>
+      <c r="P4" s="2">
+        <v>50</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>50</v>
+      </c>
+      <c r="R4" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>3000</v>
+      </c>
+      <c r="B5" s="2">
+        <v>30</v>
+      </c>
+      <c r="C5" s="2">
+        <v>36</v>
+      </c>
+      <c r="D5" s="2">
+        <v>39</v>
+      </c>
+      <c r="E5" s="2">
+        <v>39</v>
+      </c>
+      <c r="F5" s="2">
+        <v>45</v>
+      </c>
+      <c r="G5" s="2">
+        <v>45</v>
+      </c>
+      <c r="H5" s="2">
+        <v>46</v>
+      </c>
+      <c r="I5" s="2">
+        <v>48</v>
+      </c>
+      <c r="J5" s="2">
+        <v>54</v>
+      </c>
+      <c r="K5" s="2">
+        <v>57</v>
+      </c>
+      <c r="L5" s="2">
+        <v>57</v>
+      </c>
+      <c r="M5" s="2">
+        <v>60</v>
+      </c>
+      <c r="N5" s="2">
+        <v>60</v>
+      </c>
+      <c r="O5" s="2">
+        <v>60</v>
+      </c>
+      <c r="P5" s="2">
+        <v>60</v>
+      </c>
+      <c r="Q5" s="2">
+        <v>60</v>
+      </c>
+      <c r="R5" s="2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>3500</v>
+      </c>
+      <c r="B6" s="2">
+        <f>3.5*B2</f>
+        <v>35</v>
+      </c>
+      <c r="C6" s="2">
+        <f>3.5*C2</f>
+        <v>42</v>
+      </c>
+      <c r="D6" s="2">
+        <v>46</v>
+      </c>
+      <c r="E6" s="2">
+        <v>46</v>
+      </c>
+      <c r="F6" s="2">
+        <v>53</v>
+      </c>
+      <c r="G6" s="2">
+        <v>53</v>
+      </c>
+      <c r="H6" s="2">
+        <v>54</v>
+      </c>
+      <c r="I6" s="2">
+        <f>3.5*I2</f>
+        <v>56</v>
+      </c>
+      <c r="J6" s="2">
+        <f>3.5*J2</f>
+        <v>63</v>
+      </c>
+      <c r="K6" s="2">
+        <v>67</v>
+      </c>
+      <c r="L6" s="2">
+        <v>67</v>
+      </c>
+      <c r="M6" s="2">
+        <f t="shared" ref="M6:R6" si="1">3.5*M2</f>
+        <v>70</v>
+      </c>
+      <c r="N6" s="2">
+        <f t="shared" si="1"/>
+        <v>70</v>
+      </c>
+      <c r="O6" s="2">
+        <f t="shared" si="1"/>
+        <v>70</v>
+      </c>
+      <c r="P6" s="2">
+        <f t="shared" si="1"/>
+        <v>70</v>
+      </c>
+      <c r="Q6" s="2">
+        <f t="shared" si="1"/>
+        <v>70</v>
+      </c>
+      <c r="R6" s="2">
+        <f t="shared" si="1"/>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>4000</v>
+      </c>
+      <c r="B7" s="2">
+        <f t="shared" ref="B7:R7" si="2">4*B2</f>
+        <v>40</v>
+      </c>
+      <c r="C7" s="2">
+        <f t="shared" si="2"/>
+        <v>48</v>
+      </c>
+      <c r="D7" s="2">
+        <f t="shared" si="2"/>
+        <v>52</v>
+      </c>
+      <c r="E7" s="2">
+        <f t="shared" si="2"/>
+        <v>52</v>
+      </c>
+      <c r="F7" s="2">
+        <f t="shared" si="2"/>
+        <v>60</v>
+      </c>
+      <c r="G7" s="2">
+        <f t="shared" si="2"/>
+        <v>60</v>
+      </c>
+      <c r="H7" s="2">
+        <f t="shared" si="2"/>
+        <v>62</v>
+      </c>
+      <c r="I7" s="2">
+        <f t="shared" si="2"/>
+        <v>64</v>
+      </c>
+      <c r="J7" s="2">
+        <f t="shared" si="2"/>
+        <v>72</v>
+      </c>
+      <c r="K7" s="2">
+        <f t="shared" si="2"/>
+        <v>76</v>
+      </c>
+      <c r="L7" s="2">
+        <f t="shared" si="2"/>
+        <v>76</v>
+      </c>
+      <c r="M7" s="2">
+        <f t="shared" si="2"/>
+        <v>80</v>
+      </c>
+      <c r="N7" s="2">
+        <f t="shared" si="2"/>
+        <v>80</v>
+      </c>
+      <c r="O7" s="2">
+        <f t="shared" si="2"/>
+        <v>80</v>
+      </c>
+      <c r="P7" s="2">
+        <f t="shared" si="2"/>
+        <v>80</v>
+      </c>
+      <c r="Q7" s="2">
+        <f t="shared" si="2"/>
+        <v>80</v>
+      </c>
+      <c r="R7" s="2">
+        <f t="shared" si="2"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>5000</v>
+      </c>
+      <c r="B8" s="2">
+        <v>50</v>
+      </c>
+      <c r="C8" s="2">
+        <v>60</v>
+      </c>
+      <c r="D8" s="2">
+        <v>65</v>
+      </c>
+      <c r="E8" s="2">
+        <v>65</v>
+      </c>
+      <c r="F8" s="2">
+        <v>75</v>
+      </c>
+      <c r="G8" s="2">
+        <v>75</v>
+      </c>
+      <c r="H8" s="2">
+        <v>77</v>
+      </c>
+      <c r="I8" s="2">
+        <v>80</v>
+      </c>
+      <c r="J8" s="2">
+        <f>(0.018*M8)/0.02</f>
+        <v>89.999999999999986</v>
+      </c>
+      <c r="K8" s="2">
+        <f>(0.019*M8)/0.02</f>
+        <v>95</v>
+      </c>
+      <c r="L8" s="2">
+        <v>95</v>
+      </c>
+      <c r="M8" s="2">
+        <v>100</v>
+      </c>
+      <c r="N8" s="2">
+        <v>100</v>
+      </c>
+      <c r="O8" s="2">
+        <v>100</v>
+      </c>
+      <c r="P8" s="2">
+        <v>100</v>
+      </c>
+      <c r="Q8" s="2">
+        <v>100</v>
+      </c>
+      <c r="R8" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>6000</v>
+      </c>
+      <c r="B9" s="2">
+        <f t="shared" ref="B9:R9" si="3">6*B2</f>
+        <v>60</v>
+      </c>
+      <c r="C9" s="2">
+        <f t="shared" si="3"/>
+        <v>72</v>
+      </c>
+      <c r="D9" s="2">
+        <f t="shared" si="3"/>
+        <v>78</v>
+      </c>
+      <c r="E9" s="2">
+        <f t="shared" si="3"/>
+        <v>78</v>
+      </c>
+      <c r="F9" s="2">
+        <f t="shared" si="3"/>
+        <v>90</v>
+      </c>
+      <c r="G9" s="2">
+        <f t="shared" si="3"/>
+        <v>90</v>
+      </c>
+      <c r="H9" s="2">
+        <f t="shared" si="3"/>
+        <v>93</v>
+      </c>
+      <c r="I9" s="2">
+        <f t="shared" si="3"/>
+        <v>96</v>
+      </c>
+      <c r="J9" s="2">
+        <f t="shared" si="3"/>
+        <v>108</v>
+      </c>
+      <c r="K9" s="2">
+        <f t="shared" si="3"/>
+        <v>114</v>
+      </c>
+      <c r="L9" s="2">
+        <f t="shared" si="3"/>
+        <v>114</v>
+      </c>
+      <c r="M9" s="2">
+        <f t="shared" si="3"/>
+        <v>120</v>
+      </c>
+      <c r="N9" s="2">
+        <f t="shared" si="3"/>
+        <v>120</v>
+      </c>
+      <c r="O9" s="2">
+        <f t="shared" si="3"/>
+        <v>120</v>
+      </c>
+      <c r="P9" s="2">
+        <f t="shared" si="3"/>
+        <v>120</v>
+      </c>
+      <c r="Q9" s="2">
+        <f t="shared" si="3"/>
+        <v>120</v>
+      </c>
+      <c r="R9" s="2">
+        <f t="shared" si="3"/>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>7500</v>
+      </c>
+      <c r="B10" s="2">
+        <v>75</v>
+      </c>
+      <c r="C10" s="2">
+        <v>90</v>
+      </c>
+      <c r="D10" s="2">
+        <v>97</v>
+      </c>
+      <c r="E10" s="2">
+        <v>97</v>
+      </c>
+      <c r="F10" s="2">
+        <v>112</v>
+      </c>
+      <c r="G10" s="2">
+        <v>112</v>
+      </c>
+      <c r="H10" s="2">
+        <v>116</v>
+      </c>
+      <c r="I10" s="2">
+        <v>120</v>
+      </c>
+      <c r="J10" s="2">
+        <f>(0.018*M10)/0.02</f>
+        <v>134.99999999999997</v>
+      </c>
+      <c r="K10" s="2">
+        <v>142</v>
+      </c>
+      <c r="L10" s="2">
+        <v>142</v>
+      </c>
+      <c r="M10" s="2">
+        <v>150</v>
+      </c>
+      <c r="N10" s="2">
+        <v>150</v>
+      </c>
+      <c r="O10" s="2">
+        <v>150</v>
+      </c>
+      <c r="P10" s="2">
+        <v>150</v>
+      </c>
+      <c r="Q10" s="2">
+        <v>150</v>
+      </c>
+      <c r="R10" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>8000</v>
+      </c>
+      <c r="B11" s="2">
+        <f t="shared" ref="B11:R11" si="4">8*B2</f>
+        <v>80</v>
+      </c>
+      <c r="C11" s="2">
+        <f t="shared" si="4"/>
+        <v>96</v>
+      </c>
+      <c r="D11" s="2">
+        <f t="shared" si="4"/>
+        <v>104</v>
+      </c>
+      <c r="E11" s="2">
+        <f t="shared" si="4"/>
+        <v>104</v>
+      </c>
+      <c r="F11" s="2">
+        <f t="shared" si="4"/>
+        <v>120</v>
+      </c>
+      <c r="G11" s="2">
+        <f t="shared" si="4"/>
+        <v>120</v>
+      </c>
+      <c r="H11" s="2">
+        <f t="shared" si="4"/>
+        <v>124</v>
+      </c>
+      <c r="I11" s="2">
+        <f t="shared" si="4"/>
+        <v>128</v>
+      </c>
+      <c r="J11" s="2">
+        <f t="shared" si="4"/>
+        <v>144</v>
+      </c>
+      <c r="K11" s="2">
+        <f t="shared" si="4"/>
+        <v>152</v>
+      </c>
+      <c r="L11" s="2">
+        <f t="shared" si="4"/>
+        <v>152</v>
+      </c>
+      <c r="M11" s="2">
+        <f t="shared" si="4"/>
+        <v>160</v>
+      </c>
+      <c r="N11" s="2">
+        <f t="shared" si="4"/>
+        <v>160</v>
+      </c>
+      <c r="O11" s="2">
+        <f t="shared" si="4"/>
+        <v>160</v>
+      </c>
+      <c r="P11" s="2">
+        <f t="shared" si="4"/>
+        <v>160</v>
+      </c>
+      <c r="Q11" s="2">
+        <f t="shared" si="4"/>
+        <v>160</v>
+      </c>
+      <c r="R11" s="2">
+        <f t="shared" si="4"/>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>10000</v>
+      </c>
+      <c r="B12" s="2">
+        <v>100</v>
+      </c>
+      <c r="C12" s="2">
+        <v>120</v>
+      </c>
+      <c r="D12" s="2">
+        <v>130</v>
+      </c>
+      <c r="E12" s="2">
+        <v>130</v>
+      </c>
+      <c r="F12" s="2">
+        <v>150</v>
+      </c>
+      <c r="G12" s="2">
+        <v>150</v>
+      </c>
+      <c r="H12" s="2">
+        <v>155</v>
+      </c>
+      <c r="I12" s="2">
+        <v>160</v>
+      </c>
+      <c r="J12" s="2">
+        <f>(0.018*M12)/0.02</f>
+        <v>179.99999999999997</v>
+      </c>
+      <c r="K12" s="2">
+        <f>(0.019*M12)/0.02</f>
+        <v>190</v>
+      </c>
+      <c r="L12" s="2">
+        <v>190</v>
+      </c>
+      <c r="M12" s="2">
+        <v>200</v>
+      </c>
+      <c r="N12" s="2">
+        <v>200</v>
+      </c>
+      <c r="O12" s="2">
+        <v>200</v>
+      </c>
+      <c r="P12" s="2">
+        <v>200</v>
+      </c>
+      <c r="Q12" s="2">
+        <v>200</v>
+      </c>
+      <c r="R12" s="2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>12500</v>
+      </c>
+      <c r="B13" s="2">
+        <v>125</v>
+      </c>
+      <c r="C13" s="2">
+        <v>150</v>
+      </c>
+      <c r="D13" s="2">
+        <v>162</v>
+      </c>
+      <c r="E13" s="2">
+        <v>162</v>
+      </c>
+      <c r="F13" s="2">
+        <v>187</v>
+      </c>
+      <c r="G13" s="2">
+        <v>187</v>
+      </c>
+      <c r="H13" s="2">
+        <v>194</v>
+      </c>
+      <c r="I13" s="2">
+        <v>200</v>
+      </c>
+      <c r="J13" s="2">
+        <f>(0.018*M13)/0.02</f>
+        <v>225</v>
+      </c>
+      <c r="K13" s="2">
+        <v>237</v>
+      </c>
+      <c r="L13" s="2">
+        <v>237</v>
+      </c>
+      <c r="M13" s="2">
+        <v>250</v>
+      </c>
+      <c r="N13" s="2">
+        <v>250</v>
+      </c>
+      <c r="O13" s="2">
+        <v>250</v>
+      </c>
+      <c r="P13" s="2">
+        <v>250</v>
+      </c>
+      <c r="Q13" s="2">
+        <v>250</v>
+      </c>
+      <c r="R13" s="2">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>15000</v>
+      </c>
+      <c r="B14" s="2">
+        <v>150</v>
+      </c>
+      <c r="C14" s="2">
+        <v>180</v>
+      </c>
+      <c r="D14" s="2">
+        <v>195</v>
+      </c>
+      <c r="E14" s="2">
+        <v>195</v>
+      </c>
+      <c r="F14" s="2">
+        <v>225</v>
+      </c>
+      <c r="G14" s="2">
+        <v>225</v>
+      </c>
+      <c r="H14" s="2">
+        <v>233</v>
+      </c>
+      <c r="I14" s="2">
+        <v>240</v>
+      </c>
+      <c r="J14" s="2">
+        <f>(0.018*M14)/0.02</f>
+        <v>269.99999999999994</v>
+      </c>
+      <c r="K14" s="2">
+        <f>(0.019*M14)/0.02</f>
+        <v>285</v>
+      </c>
+      <c r="L14" s="2">
+        <v>285</v>
+      </c>
+      <c r="M14" s="2">
+        <v>300</v>
+      </c>
+      <c r="N14" s="2">
+        <v>300</v>
+      </c>
+      <c r="O14" s="2">
+        <v>300</v>
+      </c>
+      <c r="P14" s="2">
+        <v>300</v>
+      </c>
+      <c r="Q14" s="2">
+        <v>300</v>
+      </c>
+      <c r="R14" s="2">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>20000</v>
+      </c>
+      <c r="B15" s="2">
+        <v>175</v>
+      </c>
+      <c r="C15" s="2">
+        <v>210</v>
+      </c>
+      <c r="D15" s="2">
+        <v>227</v>
+      </c>
+      <c r="E15" s="2">
+        <v>227</v>
+      </c>
+      <c r="F15" s="2">
+        <v>262</v>
+      </c>
+      <c r="G15" s="2">
+        <v>262</v>
+      </c>
+      <c r="H15" s="2">
+        <v>271</v>
+      </c>
+      <c r="I15" s="2">
+        <v>280</v>
+      </c>
+      <c r="J15" s="2">
+        <f>(0.018*M15)/0.02</f>
+        <v>315</v>
+      </c>
+      <c r="K15" s="2">
+        <v>332</v>
+      </c>
+      <c r="L15" s="2">
+        <v>332</v>
+      </c>
+      <c r="M15" s="2">
+        <v>350</v>
+      </c>
+      <c r="N15" s="2">
+        <v>350</v>
+      </c>
+      <c r="O15" s="2">
+        <v>350</v>
+      </c>
+      <c r="P15" s="2">
+        <v>350</v>
+      </c>
+      <c r="Q15" s="2">
+        <v>350</v>
+      </c>
+      <c r="R15" s="2">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>25000</v>
+      </c>
+      <c r="B16" s="2">
+        <f t="shared" ref="B16:R16" si="5">25*B2</f>
+        <v>250</v>
+      </c>
+      <c r="C16" s="2">
+        <f t="shared" si="5"/>
+        <v>300</v>
+      </c>
+      <c r="D16" s="2">
+        <f t="shared" si="5"/>
+        <v>325</v>
+      </c>
+      <c r="E16" s="2">
+        <f t="shared" si="5"/>
+        <v>325</v>
+      </c>
+      <c r="F16" s="2">
+        <f t="shared" si="5"/>
+        <v>375</v>
+      </c>
+      <c r="G16" s="2">
+        <f t="shared" si="5"/>
+        <v>375</v>
+      </c>
+      <c r="H16" s="2">
+        <f t="shared" si="5"/>
+        <v>387.5</v>
+      </c>
+      <c r="I16" s="2">
+        <f t="shared" si="5"/>
+        <v>400</v>
+      </c>
+      <c r="J16" s="2">
+        <f t="shared" si="5"/>
+        <v>450</v>
+      </c>
+      <c r="K16" s="2">
+        <f t="shared" si="5"/>
+        <v>475</v>
+      </c>
+      <c r="L16" s="2">
+        <f t="shared" si="5"/>
+        <v>475</v>
+      </c>
+      <c r="M16" s="2">
+        <f t="shared" si="5"/>
+        <v>500</v>
+      </c>
+      <c r="N16" s="2">
+        <f t="shared" si="5"/>
+        <v>500</v>
+      </c>
+      <c r="O16" s="2">
+        <f t="shared" si="5"/>
+        <v>500</v>
+      </c>
+      <c r="P16" s="2">
+        <f t="shared" si="5"/>
+        <v>500</v>
+      </c>
+      <c r="Q16" s="2">
+        <f t="shared" si="5"/>
+        <v>500</v>
+      </c>
+      <c r="R16" s="2">
+        <f t="shared" si="5"/>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>30000</v>
+      </c>
+      <c r="B17" s="2">
+        <f t="shared" ref="B17:R17" si="6">30*B2</f>
+        <v>300</v>
+      </c>
+      <c r="C17" s="2">
+        <f t="shared" si="6"/>
+        <v>360</v>
+      </c>
+      <c r="D17" s="2">
+        <f t="shared" si="6"/>
+        <v>390</v>
+      </c>
+      <c r="E17" s="2">
+        <f t="shared" si="6"/>
+        <v>390</v>
+      </c>
+      <c r="F17" s="2">
+        <f t="shared" si="6"/>
+        <v>450</v>
+      </c>
+      <c r="G17" s="2">
+        <f t="shared" si="6"/>
+        <v>450</v>
+      </c>
+      <c r="H17" s="2">
+        <f t="shared" si="6"/>
+        <v>465</v>
+      </c>
+      <c r="I17" s="2">
+        <f t="shared" si="6"/>
+        <v>480</v>
+      </c>
+      <c r="J17" s="2">
+        <f t="shared" si="6"/>
+        <v>540</v>
+      </c>
+      <c r="K17" s="2">
+        <f t="shared" si="6"/>
+        <v>570</v>
+      </c>
+      <c r="L17" s="2">
+        <f t="shared" si="6"/>
+        <v>570</v>
+      </c>
+      <c r="M17" s="2">
+        <f t="shared" si="6"/>
+        <v>600</v>
+      </c>
+      <c r="N17" s="2">
+        <f t="shared" si="6"/>
+        <v>600</v>
+      </c>
+      <c r="O17" s="2">
+        <f t="shared" si="6"/>
+        <v>600</v>
+      </c>
+      <c r="P17" s="2">
+        <f t="shared" si="6"/>
+        <v>600</v>
+      </c>
+      <c r="Q17" s="2">
+        <f t="shared" si="6"/>
+        <v>600</v>
+      </c>
+      <c r="R17" s="2">
+        <f t="shared" si="6"/>
+        <v>600</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>40000</v>
+      </c>
+      <c r="B18" s="2">
+        <f t="shared" ref="B18:R18" si="7">2*B15</f>
+        <v>350</v>
+      </c>
+      <c r="C18" s="2">
+        <f t="shared" si="7"/>
+        <v>420</v>
+      </c>
+      <c r="D18" s="2">
+        <f t="shared" si="7"/>
+        <v>454</v>
+      </c>
+      <c r="E18" s="2">
+        <f t="shared" si="7"/>
+        <v>454</v>
+      </c>
+      <c r="F18" s="2">
+        <f t="shared" si="7"/>
+        <v>524</v>
+      </c>
+      <c r="G18" s="2">
+        <f t="shared" si="7"/>
+        <v>524</v>
+      </c>
+      <c r="H18" s="2">
+        <f t="shared" si="7"/>
+        <v>542</v>
+      </c>
+      <c r="I18" s="2">
+        <f t="shared" si="7"/>
+        <v>560</v>
+      </c>
+      <c r="J18" s="2">
+        <f t="shared" si="7"/>
+        <v>630</v>
+      </c>
+      <c r="K18" s="2">
+        <f t="shared" si="7"/>
+        <v>664</v>
+      </c>
+      <c r="L18" s="2">
+        <f t="shared" si="7"/>
+        <v>664</v>
+      </c>
+      <c r="M18" s="2">
+        <f t="shared" si="7"/>
+        <v>700</v>
+      </c>
+      <c r="N18" s="2">
+        <f t="shared" si="7"/>
+        <v>700</v>
+      </c>
+      <c r="O18" s="2">
+        <f t="shared" si="7"/>
+        <v>700</v>
+      </c>
+      <c r="P18" s="2">
+        <f t="shared" si="7"/>
+        <v>700</v>
+      </c>
+      <c r="Q18" s="2">
+        <f t="shared" si="7"/>
+        <v>700</v>
+      </c>
+      <c r="R18" s="2">
+        <f t="shared" si="7"/>
+        <v>700</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:R18"/>
   <sheetViews>

</xml_diff>

<commit_message>
Fixed: - add module edit money paid Thu ve, chot, be
</commit_message>
<xml_diff>
--- a/dev/cuahang.xlsx
+++ b/dev/cuahang.xlsx
@@ -1590,7 +1590,7 @@
   <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1660,67 +1660,55 @@
         <v>1000</v>
       </c>
       <c r="B2" s="2">
-        <f t="shared" ref="B2:M2" si="0">0.5*B3</f>
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="C2" s="2">
-        <f t="shared" si="0"/>
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="D2" s="2">
-        <f t="shared" si="0"/>
-        <v>45</v>
+        <v>13</v>
       </c>
       <c r="E2" s="2">
-        <f t="shared" si="0"/>
-        <v>47</v>
+        <v>13</v>
       </c>
       <c r="F2" s="2">
-        <f t="shared" si="0"/>
-        <v>51</v>
+        <v>15</v>
       </c>
       <c r="G2" s="2">
-        <f t="shared" si="0"/>
-        <v>53</v>
+        <v>15</v>
       </c>
       <c r="H2" s="2">
-        <f t="shared" si="0"/>
-        <v>55</v>
+        <v>15.5</v>
       </c>
       <c r="I2" s="2">
-        <f t="shared" si="0"/>
-        <v>57</v>
+        <v>16</v>
       </c>
       <c r="J2" s="2">
-        <f t="shared" si="0"/>
-        <v>64</v>
+        <v>18</v>
       </c>
       <c r="K2" s="2">
-        <f t="shared" si="0"/>
-        <v>66</v>
+        <v>19</v>
       </c>
       <c r="L2" s="2">
-        <f t="shared" si="0"/>
-        <v>68</v>
+        <v>19</v>
       </c>
       <c r="M2" s="2">
-        <f t="shared" si="0"/>
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="N2" s="2">
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="O2" s="2">
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="P2" s="2">
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="Q2" s="2">
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="R2" s="2">
-        <v>70</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="16" x14ac:dyDescent="0.2">
@@ -1728,55 +1716,55 @@
         <v>2000</v>
       </c>
       <c r="B3" s="2">
-        <v>64</v>
+        <v>20</v>
       </c>
       <c r="C3" s="2">
-        <v>84</v>
+        <v>24</v>
       </c>
       <c r="D3" s="2">
-        <v>90</v>
+        <v>26</v>
       </c>
       <c r="E3" s="2">
-        <v>94</v>
+        <v>26</v>
       </c>
       <c r="F3" s="2">
-        <v>102</v>
+        <v>30</v>
       </c>
       <c r="G3" s="2">
-        <v>106</v>
+        <v>30</v>
       </c>
       <c r="H3" s="2">
-        <v>110</v>
+        <v>31</v>
       </c>
       <c r="I3" s="2">
-        <v>114</v>
+        <v>32</v>
       </c>
       <c r="J3" s="2">
-        <v>128</v>
+        <v>36</v>
       </c>
       <c r="K3" s="2">
-        <v>132</v>
+        <v>38</v>
       </c>
       <c r="L3" s="2">
-        <v>136</v>
+        <v>38</v>
       </c>
       <c r="M3" s="2">
-        <v>140</v>
+        <v>40</v>
       </c>
       <c r="N3" s="2">
-        <v>140</v>
+        <v>40</v>
       </c>
       <c r="O3" s="2">
-        <v>140</v>
+        <v>40</v>
       </c>
       <c r="P3" s="2">
-        <v>140</v>
+        <v>40</v>
       </c>
       <c r="Q3" s="2">
-        <v>140</v>
+        <v>40</v>
       </c>
       <c r="R3" s="2">
-        <v>140</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="16" x14ac:dyDescent="0.2">
@@ -1784,57 +1772,55 @@
         <v>2500</v>
       </c>
       <c r="B4" s="2">
-        <v>80</v>
+        <v>25</v>
       </c>
       <c r="C4" s="2">
-        <v>105</v>
+        <v>30</v>
       </c>
       <c r="D4" s="2">
-        <v>112</v>
+        <v>32</v>
       </c>
       <c r="E4" s="2">
-        <v>117</v>
+        <v>32</v>
       </c>
       <c r="F4" s="2">
-        <v>127</v>
+        <v>37</v>
       </c>
       <c r="G4" s="2">
-        <v>132</v>
+        <v>37</v>
       </c>
       <c r="H4" s="2">
-        <v>138</v>
+        <v>38</v>
       </c>
       <c r="I4" s="2">
-        <v>142</v>
+        <v>40</v>
       </c>
       <c r="J4" s="2">
-        <f>(0.064*M4)/0.07</f>
-        <v>160</v>
+        <v>44.999999999999993</v>
       </c>
       <c r="K4" s="2">
-        <f>(0.066*M4)/0.07</f>
-        <v>165</v>
+        <v>47</v>
       </c>
       <c r="L4" s="2">
-        <v>170</v>
+        <v>47</v>
       </c>
       <c r="M4" s="2">
-        <v>175</v>
+        <v>50</v>
       </c>
       <c r="N4" s="2">
-        <v>175</v>
+        <v>50</v>
       </c>
       <c r="O4" s="2">
-        <v>175</v>
+        <v>50</v>
       </c>
       <c r="P4" s="2">
-        <v>175</v>
+        <v>50</v>
       </c>
       <c r="Q4" s="2">
-        <v>175</v>
+        <v>50</v>
       </c>
       <c r="R4" s="2">
-        <v>175</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="16" x14ac:dyDescent="0.2">
@@ -1842,55 +1828,55 @@
         <v>3000</v>
       </c>
       <c r="B5" s="2">
-        <v>96</v>
+        <v>30</v>
       </c>
       <c r="C5" s="2">
-        <v>126</v>
+        <v>36</v>
       </c>
       <c r="D5" s="2">
-        <v>134</v>
+        <v>39</v>
       </c>
       <c r="E5" s="2">
-        <v>140</v>
+        <v>39</v>
       </c>
       <c r="F5" s="2">
-        <v>152</v>
+        <v>45</v>
       </c>
       <c r="G5" s="2">
-        <v>158</v>
+        <v>45</v>
       </c>
       <c r="H5" s="2">
-        <v>165</v>
+        <v>46</v>
       </c>
       <c r="I5" s="2">
-        <v>170</v>
+        <v>48</v>
       </c>
       <c r="J5" s="2">
-        <v>192</v>
+        <v>54</v>
       </c>
       <c r="K5" s="2">
-        <v>198</v>
+        <v>57</v>
       </c>
       <c r="L5" s="2">
-        <v>204</v>
+        <v>57</v>
       </c>
       <c r="M5" s="2">
-        <v>210</v>
+        <v>60</v>
       </c>
       <c r="N5" s="2">
-        <v>210</v>
+        <v>60</v>
       </c>
       <c r="O5" s="2">
-        <v>210</v>
+        <v>60</v>
       </c>
       <c r="P5" s="2">
-        <v>210</v>
+        <v>60</v>
       </c>
       <c r="Q5" s="2">
-        <v>210</v>
+        <v>60</v>
       </c>
       <c r="R5" s="2">
-        <v>210</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="16" x14ac:dyDescent="0.2">
@@ -1898,66 +1884,55 @@
         <v>3500</v>
       </c>
       <c r="B6" s="2">
-        <f>3.5*B2</f>
-        <v>112</v>
+        <v>35</v>
       </c>
       <c r="C6" s="2">
-        <f>3.5*C2</f>
-        <v>147</v>
+        <v>42</v>
       </c>
       <c r="D6" s="2">
-        <v>158</v>
+        <v>46</v>
       </c>
       <c r="E6" s="2">
-        <v>165</v>
+        <v>46</v>
       </c>
       <c r="F6" s="2">
-        <v>179</v>
+        <v>53</v>
       </c>
       <c r="G6" s="2">
-        <v>186</v>
+        <v>53</v>
       </c>
       <c r="H6" s="2">
-        <v>193</v>
+        <v>54</v>
       </c>
       <c r="I6" s="2">
-        <v>200</v>
+        <v>56</v>
       </c>
       <c r="J6" s="2">
-        <f t="shared" ref="J6:R6" si="1">3.5*J2</f>
-        <v>224</v>
+        <v>63</v>
       </c>
       <c r="K6" s="2">
-        <f t="shared" si="1"/>
-        <v>231</v>
+        <v>67</v>
       </c>
       <c r="L6" s="2">
-        <f t="shared" si="1"/>
-        <v>238</v>
+        <v>67</v>
       </c>
       <c r="M6" s="2">
-        <f t="shared" si="1"/>
-        <v>245</v>
+        <v>70</v>
       </c>
       <c r="N6" s="2">
-        <f t="shared" si="1"/>
-        <v>245</v>
+        <v>70</v>
       </c>
       <c r="O6" s="2">
-        <f t="shared" si="1"/>
-        <v>245</v>
+        <v>70</v>
       </c>
       <c r="P6" s="2">
-        <f t="shared" si="1"/>
-        <v>245</v>
+        <v>70</v>
       </c>
       <c r="Q6" s="2">
-        <f t="shared" si="1"/>
-        <v>245</v>
+        <v>70</v>
       </c>
       <c r="R6" s="2">
-        <f t="shared" si="1"/>
-        <v>245</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="16" x14ac:dyDescent="0.2">
@@ -1965,70 +1940,55 @@
         <v>4000</v>
       </c>
       <c r="B7" s="2">
-        <f>($A$7/$A$3)*B3</f>
-        <v>128</v>
+        <v>40</v>
       </c>
       <c r="C7" s="2">
-        <f>2*84</f>
-        <v>168</v>
+        <v>48</v>
       </c>
       <c r="D7" s="2">
-        <v>180</v>
+        <v>52</v>
       </c>
       <c r="E7" s="2">
-        <f>94*2</f>
-        <v>188</v>
+        <v>52</v>
       </c>
       <c r="F7" s="2">
-        <f>102*2</f>
-        <v>204</v>
+        <v>60</v>
       </c>
       <c r="G7" s="2">
-        <f>(A7/A3)*G3</f>
-        <v>212</v>
+        <v>60</v>
       </c>
       <c r="H7" s="2">
-        <v>220</v>
+        <v>62</v>
       </c>
       <c r="I7" s="2">
-        <f>114*2</f>
-        <v>228</v>
+        <v>64</v>
       </c>
       <c r="J7" s="2">
-        <f>128*2</f>
-        <v>256</v>
+        <v>72</v>
       </c>
       <c r="K7" s="2">
-        <f>132*2</f>
-        <v>264</v>
+        <v>76</v>
       </c>
       <c r="L7" s="2">
-        <f>136*2</f>
-        <v>272</v>
+        <v>76</v>
       </c>
       <c r="M7" s="2">
-        <f t="shared" ref="M7:R7" si="2">140*2</f>
-        <v>280</v>
+        <v>80</v>
       </c>
       <c r="N7" s="2">
-        <f t="shared" si="2"/>
-        <v>280</v>
+        <v>80</v>
       </c>
       <c r="O7" s="2">
-        <f t="shared" si="2"/>
-        <v>280</v>
+        <v>80</v>
       </c>
       <c r="P7" s="2">
-        <f t="shared" si="2"/>
-        <v>280</v>
+        <v>80</v>
       </c>
       <c r="Q7" s="2">
-        <f t="shared" si="2"/>
-        <v>280</v>
+        <v>80</v>
       </c>
       <c r="R7" s="2">
-        <f t="shared" si="2"/>
-        <v>280</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="16" x14ac:dyDescent="0.2">
@@ -2036,57 +1996,55 @@
         <v>5000</v>
       </c>
       <c r="B8" s="2">
-        <v>160</v>
+        <v>50</v>
       </c>
       <c r="C8" s="2">
-        <v>210</v>
+        <v>60</v>
       </c>
       <c r="D8" s="2">
-        <v>225</v>
+        <v>65</v>
       </c>
       <c r="E8" s="2">
-        <v>235</v>
+        <v>65</v>
       </c>
       <c r="F8" s="2">
-        <v>255</v>
+        <v>75</v>
       </c>
       <c r="G8" s="2">
-        <v>265</v>
+        <v>75</v>
       </c>
       <c r="H8" s="2">
-        <v>275</v>
+        <v>77</v>
       </c>
       <c r="I8" s="2">
-        <v>285</v>
+        <v>80</v>
       </c>
       <c r="J8" s="2">
-        <f>(0.064*M8)/0.07</f>
-        <v>320</v>
+        <v>89.999999999999986</v>
       </c>
       <c r="K8" s="2">
-        <f>(0.066*M8)/0.07</f>
-        <v>330</v>
+        <v>95</v>
       </c>
       <c r="L8" s="2">
-        <v>340</v>
+        <v>95</v>
       </c>
       <c r="M8" s="2">
-        <v>350</v>
+        <v>100</v>
       </c>
       <c r="N8" s="2">
-        <v>350</v>
+        <v>100</v>
       </c>
       <c r="O8" s="2">
-        <v>350</v>
+        <v>100</v>
       </c>
       <c r="P8" s="2">
-        <v>350</v>
+        <v>100</v>
       </c>
       <c r="Q8" s="2">
-        <v>350</v>
+        <v>100</v>
       </c>
       <c r="R8" s="2">
-        <v>350</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="16" x14ac:dyDescent="0.2">
@@ -2094,72 +2052,55 @@
         <v>6000</v>
       </c>
       <c r="B9" s="2">
-        <f>3*64</f>
-        <v>192</v>
+        <v>60</v>
       </c>
       <c r="C9" s="2">
-        <f>3*84</f>
-        <v>252</v>
+        <v>72</v>
       </c>
       <c r="D9" s="2">
-        <f t="shared" ref="D9:L9" si="3">3*D3</f>
-        <v>270</v>
+        <v>78</v>
       </c>
       <c r="E9" s="2">
-        <f t="shared" si="3"/>
-        <v>282</v>
+        <v>78</v>
       </c>
       <c r="F9" s="2">
-        <f t="shared" si="3"/>
-        <v>306</v>
+        <v>90</v>
       </c>
       <c r="G9" s="2">
-        <f t="shared" si="3"/>
-        <v>318</v>
+        <v>90</v>
       </c>
       <c r="H9" s="2">
-        <f t="shared" si="3"/>
-        <v>330</v>
+        <v>93</v>
       </c>
       <c r="I9" s="2">
-        <f t="shared" si="3"/>
-        <v>342</v>
+        <v>96</v>
       </c>
       <c r="J9" s="2">
-        <f t="shared" si="3"/>
-        <v>384</v>
+        <v>108</v>
       </c>
       <c r="K9" s="2">
-        <f t="shared" si="3"/>
-        <v>396</v>
+        <v>114</v>
       </c>
       <c r="L9" s="2">
-        <f t="shared" si="3"/>
-        <v>408</v>
+        <v>114</v>
       </c>
       <c r="M9" s="2">
-        <f t="shared" ref="M9:R9" si="4">3*140</f>
-        <v>420</v>
+        <v>120</v>
       </c>
       <c r="N9" s="2">
-        <f t="shared" si="4"/>
-        <v>420</v>
+        <v>120</v>
       </c>
       <c r="O9" s="2">
-        <f t="shared" si="4"/>
-        <v>420</v>
+        <v>120</v>
       </c>
       <c r="P9" s="2">
-        <f t="shared" si="4"/>
-        <v>420</v>
+        <v>120</v>
       </c>
       <c r="Q9" s="2">
-        <f t="shared" si="4"/>
-        <v>420</v>
+        <v>120</v>
       </c>
       <c r="R9" s="2">
-        <f t="shared" si="4"/>
-        <v>420</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="16" x14ac:dyDescent="0.2">
@@ -2167,57 +2108,55 @@
         <v>7500</v>
       </c>
       <c r="B10" s="2">
-        <v>240</v>
+        <v>75</v>
       </c>
       <c r="C10" s="2">
-        <v>315</v>
+        <v>90</v>
       </c>
       <c r="D10" s="2">
-        <v>337</v>
+        <v>97</v>
       </c>
       <c r="E10" s="2">
-        <v>352</v>
+        <v>97</v>
       </c>
       <c r="F10" s="2">
-        <v>382</v>
+        <v>112</v>
       </c>
       <c r="G10" s="2">
-        <v>397</v>
+        <v>112</v>
       </c>
       <c r="H10" s="2">
-        <v>412</v>
+        <v>116</v>
       </c>
       <c r="I10" s="2">
-        <v>427</v>
+        <v>120</v>
       </c>
       <c r="J10" s="2">
-        <f>(0.064*M10)/0.07</f>
-        <v>480</v>
+        <v>134.99999999999997</v>
       </c>
       <c r="K10" s="2">
-        <f>(0.066*M10)/0.07</f>
-        <v>494.99999999999994</v>
+        <v>142</v>
       </c>
       <c r="L10" s="2">
-        <v>510</v>
+        <v>142</v>
       </c>
       <c r="M10" s="2">
-        <v>525</v>
+        <v>150</v>
       </c>
       <c r="N10" s="2">
-        <v>525</v>
+        <v>150</v>
       </c>
       <c r="O10" s="2">
-        <v>525</v>
+        <v>150</v>
       </c>
       <c r="P10" s="2">
-        <v>525</v>
+        <v>150</v>
       </c>
       <c r="Q10" s="2">
-        <v>525</v>
+        <v>150</v>
       </c>
       <c r="R10" s="2">
-        <v>525</v>
+        <v>150</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="16" x14ac:dyDescent="0.2">
@@ -2225,72 +2164,55 @@
         <v>8000</v>
       </c>
       <c r="B11" s="2">
-        <f t="shared" ref="B11:R11" si="5">8*B2</f>
-        <v>256</v>
+        <v>80</v>
       </c>
       <c r="C11" s="2">
-        <f t="shared" si="5"/>
-        <v>336</v>
+        <v>96</v>
       </c>
       <c r="D11" s="2">
-        <f t="shared" si="5"/>
-        <v>360</v>
+        <v>104</v>
       </c>
       <c r="E11" s="2">
-        <f t="shared" si="5"/>
-        <v>376</v>
+        <v>104</v>
       </c>
       <c r="F11" s="2">
-        <f t="shared" si="5"/>
-        <v>408</v>
+        <v>120</v>
       </c>
       <c r="G11" s="2">
-        <f t="shared" si="5"/>
-        <v>424</v>
+        <v>120</v>
       </c>
       <c r="H11" s="2">
-        <f t="shared" si="5"/>
-        <v>440</v>
+        <v>124</v>
       </c>
       <c r="I11" s="2">
-        <f t="shared" si="5"/>
-        <v>456</v>
+        <v>128</v>
       </c>
       <c r="J11" s="2">
-        <f t="shared" si="5"/>
-        <v>512</v>
+        <v>144</v>
       </c>
       <c r="K11" s="2">
-        <f t="shared" si="5"/>
-        <v>528</v>
+        <v>152</v>
       </c>
       <c r="L11" s="2">
-        <f t="shared" si="5"/>
-        <v>544</v>
+        <v>152</v>
       </c>
       <c r="M11" s="2">
-        <f t="shared" si="5"/>
-        <v>560</v>
+        <v>160</v>
       </c>
       <c r="N11" s="2">
-        <f t="shared" si="5"/>
-        <v>560</v>
+        <v>160</v>
       </c>
       <c r="O11" s="2">
-        <f t="shared" si="5"/>
-        <v>560</v>
+        <v>160</v>
       </c>
       <c r="P11" s="2">
-        <f t="shared" si="5"/>
-        <v>560</v>
+        <v>160</v>
       </c>
       <c r="Q11" s="2">
-        <f t="shared" si="5"/>
-        <v>560</v>
+        <v>160</v>
       </c>
       <c r="R11" s="2">
-        <f t="shared" si="5"/>
-        <v>560</v>
+        <v>160</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="16" x14ac:dyDescent="0.2">
@@ -2298,57 +2220,55 @@
         <v>10000</v>
       </c>
       <c r="B12" s="2">
-        <v>320</v>
+        <v>100</v>
       </c>
       <c r="C12" s="2">
-        <v>420</v>
+        <v>120</v>
       </c>
       <c r="D12" s="2">
-        <v>450</v>
+        <v>130</v>
       </c>
       <c r="E12" s="2">
-        <v>470</v>
+        <v>130</v>
       </c>
       <c r="F12" s="2">
-        <v>510</v>
+        <v>150</v>
       </c>
       <c r="G12" s="2">
-        <v>530</v>
+        <v>150</v>
       </c>
       <c r="H12" s="2">
-        <v>550</v>
+        <v>155</v>
       </c>
       <c r="I12" s="2">
-        <v>570</v>
+        <v>160</v>
       </c>
       <c r="J12" s="2">
-        <f>(0.064*M12)/0.07</f>
-        <v>640</v>
+        <v>179.99999999999997</v>
       </c>
       <c r="K12" s="2">
-        <f>(0.066*M12)/0.07</f>
-        <v>660</v>
+        <v>190</v>
       </c>
       <c r="L12" s="2">
-        <v>680</v>
+        <v>190</v>
       </c>
       <c r="M12" s="2">
-        <v>700</v>
+        <v>200</v>
       </c>
       <c r="N12" s="2">
-        <v>700</v>
+        <v>200</v>
       </c>
       <c r="O12" s="2">
-        <v>700</v>
+        <v>200</v>
       </c>
       <c r="P12" s="2">
-        <v>700</v>
+        <v>200</v>
       </c>
       <c r="Q12" s="2">
-        <v>700</v>
+        <v>200</v>
       </c>
       <c r="R12" s="2">
-        <v>700</v>
+        <v>200</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="16" x14ac:dyDescent="0.2">
@@ -2356,57 +2276,55 @@
         <v>12500</v>
       </c>
       <c r="B13" s="2">
-        <v>400</v>
+        <v>125</v>
       </c>
       <c r="C13" s="2">
-        <v>525</v>
+        <v>150</v>
       </c>
       <c r="D13" s="2">
-        <v>562</v>
+        <v>162</v>
       </c>
       <c r="E13" s="2">
-        <v>587</v>
+        <v>162</v>
       </c>
       <c r="F13" s="2">
-        <v>637</v>
+        <v>187</v>
       </c>
       <c r="G13" s="2">
-        <v>662</v>
+        <v>187</v>
       </c>
       <c r="H13" s="2">
-        <v>687</v>
+        <v>194</v>
       </c>
       <c r="I13" s="2">
-        <v>712</v>
+        <v>200</v>
       </c>
       <c r="J13" s="2">
-        <f>(0.064*M13)/0.07</f>
-        <v>799.99999999999989</v>
+        <v>225</v>
       </c>
       <c r="K13" s="2">
-        <f>(0.066*M13)/0.07</f>
-        <v>824.99999999999989</v>
+        <v>237</v>
       </c>
       <c r="L13" s="2">
-        <v>850</v>
+        <v>237</v>
       </c>
       <c r="M13" s="2">
-        <v>875</v>
+        <v>250</v>
       </c>
       <c r="N13" s="2">
-        <v>875</v>
+        <v>250</v>
       </c>
       <c r="O13" s="2">
-        <v>875</v>
+        <v>250</v>
       </c>
       <c r="P13" s="2">
-        <v>875</v>
+        <v>250</v>
       </c>
       <c r="Q13" s="2">
-        <v>875</v>
+        <v>250</v>
       </c>
       <c r="R13" s="2">
-        <v>875</v>
+        <v>250</v>
       </c>
     </row>
     <row r="14" spans="1:18" ht="16" x14ac:dyDescent="0.2">
@@ -2414,57 +2332,55 @@
         <v>15000</v>
       </c>
       <c r="B14" s="2">
-        <v>480</v>
+        <v>150</v>
       </c>
       <c r="C14" s="2">
-        <v>630</v>
+        <v>180</v>
       </c>
       <c r="D14" s="2">
-        <v>675</v>
+        <v>195</v>
       </c>
       <c r="E14" s="2">
-        <v>705</v>
+        <v>195</v>
       </c>
       <c r="F14" s="2">
-        <v>765</v>
+        <v>225</v>
       </c>
       <c r="G14" s="2">
-        <v>795</v>
+        <v>225</v>
       </c>
       <c r="H14" s="2">
-        <v>825</v>
+        <v>233</v>
       </c>
       <c r="I14" s="2">
-        <v>855</v>
+        <v>240</v>
       </c>
       <c r="J14" s="2">
-        <f>(0.064*M14)/0.07</f>
-        <v>960</v>
+        <v>269.99999999999994</v>
       </c>
       <c r="K14" s="2">
-        <f>(0.066*M14)/0.07</f>
-        <v>989.99999999999989</v>
+        <v>285</v>
       </c>
       <c r="L14" s="2">
-        <v>1020</v>
+        <v>285</v>
       </c>
       <c r="M14" s="2">
-        <v>1050</v>
+        <v>300</v>
       </c>
       <c r="N14" s="2">
-        <v>1050</v>
+        <v>300</v>
       </c>
       <c r="O14" s="2">
-        <v>1050</v>
+        <v>300</v>
       </c>
       <c r="P14" s="2">
-        <v>1050</v>
+        <v>300</v>
       </c>
       <c r="Q14" s="2">
-        <v>1050</v>
+        <v>300</v>
       </c>
       <c r="R14" s="2">
-        <v>1050</v>
+        <v>300</v>
       </c>
     </row>
     <row r="15" spans="1:18" ht="16" x14ac:dyDescent="0.2">
@@ -2472,57 +2388,55 @@
         <v>20000</v>
       </c>
       <c r="B15" s="2">
-        <v>640</v>
+        <v>175</v>
       </c>
       <c r="C15" s="2">
-        <v>840</v>
+        <v>210</v>
       </c>
       <c r="D15" s="2">
-        <v>900</v>
+        <v>227</v>
       </c>
       <c r="E15" s="2">
-        <v>940</v>
+        <v>227</v>
       </c>
       <c r="F15" s="2">
-        <v>1020</v>
+        <v>262</v>
       </c>
       <c r="G15" s="2">
-        <v>1060</v>
+        <v>262</v>
       </c>
       <c r="H15" s="2">
-        <v>1100</v>
+        <v>271</v>
       </c>
       <c r="I15" s="2">
-        <v>1140</v>
+        <v>280</v>
       </c>
       <c r="J15" s="2">
-        <f>(0.064*M15)/0.07</f>
-        <v>1280</v>
+        <v>315</v>
       </c>
       <c r="K15" s="2">
-        <f>(0.066*M15)/0.07</f>
-        <v>1320</v>
+        <v>380</v>
       </c>
       <c r="L15" s="2">
-        <v>1360</v>
+        <v>380</v>
       </c>
       <c r="M15" s="2">
-        <v>1400</v>
+        <v>380</v>
       </c>
       <c r="N15" s="2">
-        <v>1400</v>
+        <v>400</v>
       </c>
       <c r="O15" s="2">
-        <v>1400</v>
+        <v>400</v>
       </c>
       <c r="P15" s="2">
-        <v>1400</v>
+        <v>400</v>
       </c>
       <c r="Q15" s="2">
-        <v>1400</v>
+        <v>400</v>
       </c>
       <c r="R15" s="2">
-        <v>1400</v>
+        <v>400</v>
       </c>
     </row>
     <row r="16" spans="1:18" ht="16" x14ac:dyDescent="0.2">
@@ -2530,72 +2444,55 @@
         <v>25000</v>
       </c>
       <c r="B16" s="2">
-        <f t="shared" ref="B16:R16" si="6">25*32</f>
-        <v>800</v>
+        <v>250</v>
       </c>
       <c r="C16" s="2">
-        <f t="shared" si="6"/>
-        <v>800</v>
+        <v>300</v>
       </c>
       <c r="D16" s="2">
-        <f t="shared" si="6"/>
-        <v>800</v>
+        <v>325</v>
       </c>
       <c r="E16" s="2">
-        <f t="shared" si="6"/>
-        <v>800</v>
+        <v>325</v>
       </c>
       <c r="F16" s="2">
-        <f t="shared" si="6"/>
-        <v>800</v>
+        <v>375</v>
       </c>
       <c r="G16" s="2">
-        <f t="shared" si="6"/>
-        <v>800</v>
+        <v>375</v>
       </c>
       <c r="H16" s="2">
-        <f t="shared" si="6"/>
-        <v>800</v>
+        <v>387.5</v>
       </c>
       <c r="I16" s="2">
-        <f t="shared" si="6"/>
-        <v>800</v>
+        <v>400</v>
       </c>
       <c r="J16" s="2">
-        <f t="shared" si="6"/>
-        <v>800</v>
+        <v>450</v>
       </c>
       <c r="K16" s="2">
-        <f t="shared" si="6"/>
-        <v>800</v>
+        <v>475</v>
       </c>
       <c r="L16" s="2">
-        <f t="shared" si="6"/>
-        <v>800</v>
+        <v>475</v>
       </c>
       <c r="M16" s="2">
-        <f t="shared" si="6"/>
-        <v>800</v>
+        <v>500</v>
       </c>
       <c r="N16" s="2">
-        <f t="shared" si="6"/>
-        <v>800</v>
+        <v>500</v>
       </c>
       <c r="O16" s="2">
-        <f t="shared" si="6"/>
-        <v>800</v>
+        <v>500</v>
       </c>
       <c r="P16" s="2">
-        <f t="shared" si="6"/>
-        <v>800</v>
+        <v>500</v>
       </c>
       <c r="Q16" s="2">
-        <f t="shared" si="6"/>
-        <v>800</v>
+        <v>500</v>
       </c>
       <c r="R16" s="2">
-        <f t="shared" si="6"/>
-        <v>800</v>
+        <v>500</v>
       </c>
     </row>
     <row r="17" spans="1:18" ht="16" x14ac:dyDescent="0.2">
@@ -2603,72 +2500,55 @@
         <v>30000</v>
       </c>
       <c r="B17" s="2">
-        <f t="shared" ref="B17:R17" si="7">30*B2</f>
-        <v>960</v>
+        <v>300</v>
       </c>
       <c r="C17" s="2">
-        <f t="shared" si="7"/>
-        <v>1260</v>
+        <v>360</v>
       </c>
       <c r="D17" s="2">
-        <f t="shared" si="7"/>
-        <v>1350</v>
+        <v>390</v>
       </c>
       <c r="E17" s="2">
-        <f t="shared" si="7"/>
-        <v>1410</v>
+        <v>390</v>
       </c>
       <c r="F17" s="2">
-        <f t="shared" si="7"/>
-        <v>1530</v>
+        <v>450</v>
       </c>
       <c r="G17" s="2">
-        <f t="shared" si="7"/>
-        <v>1590</v>
+        <v>450</v>
       </c>
       <c r="H17" s="2">
-        <f t="shared" si="7"/>
-        <v>1650</v>
+        <v>465</v>
       </c>
       <c r="I17" s="2">
-        <f t="shared" si="7"/>
-        <v>1710</v>
+        <v>480</v>
       </c>
       <c r="J17" s="2">
-        <f t="shared" si="7"/>
-        <v>1920</v>
+        <v>540</v>
       </c>
       <c r="K17" s="2">
-        <f t="shared" si="7"/>
-        <v>1980</v>
+        <v>570</v>
       </c>
       <c r="L17" s="2">
-        <f t="shared" si="7"/>
-        <v>2040</v>
+        <v>570</v>
       </c>
       <c r="M17" s="2">
-        <f t="shared" si="7"/>
-        <v>2100</v>
+        <v>600</v>
       </c>
       <c r="N17" s="2">
-        <f t="shared" si="7"/>
-        <v>2100</v>
+        <v>600</v>
       </c>
       <c r="O17" s="2">
-        <f t="shared" si="7"/>
-        <v>2100</v>
+        <v>600</v>
       </c>
       <c r="P17" s="2">
-        <f t="shared" si="7"/>
-        <v>2100</v>
+        <v>600</v>
       </c>
       <c r="Q17" s="2">
-        <f t="shared" si="7"/>
-        <v>2100</v>
+        <v>600</v>
       </c>
       <c r="R17" s="2">
-        <f t="shared" si="7"/>
-        <v>2100</v>
+        <v>600</v>
       </c>
     </row>
     <row r="18" spans="1:18" ht="16" x14ac:dyDescent="0.2">
@@ -2676,72 +2556,55 @@
         <v>40000</v>
       </c>
       <c r="B18" s="2">
-        <f t="shared" ref="B18:R18" si="8">2*B15</f>
-        <v>1280</v>
+        <v>350</v>
       </c>
       <c r="C18" s="2">
-        <f t="shared" si="8"/>
-        <v>1680</v>
+        <v>420</v>
       </c>
       <c r="D18" s="2">
-        <f t="shared" si="8"/>
-        <v>1800</v>
+        <v>454</v>
       </c>
       <c r="E18" s="2">
-        <f t="shared" si="8"/>
-        <v>1880</v>
+        <v>454</v>
       </c>
       <c r="F18" s="2">
-        <f t="shared" si="8"/>
-        <v>2040</v>
+        <v>524</v>
       </c>
       <c r="G18" s="2">
-        <f t="shared" si="8"/>
-        <v>2120</v>
+        <v>524</v>
       </c>
       <c r="H18" s="2">
-        <f t="shared" si="8"/>
-        <v>2200</v>
+        <v>542</v>
       </c>
       <c r="I18" s="2">
-        <f t="shared" si="8"/>
-        <v>2280</v>
+        <v>560</v>
       </c>
       <c r="J18" s="2">
-        <f t="shared" si="8"/>
-        <v>2560</v>
+        <v>630</v>
       </c>
       <c r="K18" s="2">
-        <f t="shared" si="8"/>
-        <v>2640</v>
+        <v>664</v>
       </c>
       <c r="L18" s="2">
-        <f t="shared" si="8"/>
-        <v>2720</v>
+        <v>664</v>
       </c>
       <c r="M18" s="2">
-        <f t="shared" si="8"/>
-        <v>2800</v>
+        <v>700</v>
       </c>
       <c r="N18" s="2">
-        <f t="shared" si="8"/>
-        <v>2800</v>
+        <v>700</v>
       </c>
       <c r="O18" s="2">
-        <f t="shared" si="8"/>
-        <v>2800</v>
+        <v>700</v>
       </c>
       <c r="P18" s="2">
-        <f t="shared" si="8"/>
-        <v>2800</v>
+        <v>700</v>
       </c>
       <c r="Q18" s="2">
-        <f t="shared" si="8"/>
-        <v>2800</v>
+        <v>700</v>
       </c>
       <c r="R18" s="2">
-        <f t="shared" si="8"/>
-        <v>2800</v>
+        <v>700</v>
       </c>
     </row>
   </sheetData>

</xml_diff>